<commit_message>
update flow booking price
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/IntegrationFlows_WithPriceCheck.xlsx
+++ b/src/main/resources/input_excel_file/booking/IntegrationFlows_WithPriceCheck.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13080"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="flows" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <t>{
   "price_validation": 
   [
-    {"booking_index": 0, "expected_amount": 1700000}
+    {"booking_index": 0, "expected_amount": 1500000}
   ]
 }</t>
   </si>
@@ -102,6 +102,14 @@
     <t>BB_VST_003</t>
   </si>
   <si>
+    <t>{
+  "price_validation": 
+  [
+    {"booking_index": 0, "expected_amount": 1700000}
+  ]
+}</t>
+  </si>
+  <si>
     <t>FLOW_PRICE_004</t>
   </si>
   <si>
@@ -154,14 +162,6 @@
     <t>BB_VST_007</t>
   </si>
   <si>
-    <t>{
-  "price_validation": 
-  [
-    {"booking_index": 0, "expected_amount": 1500000}
-  ]
-}</t>
-  </si>
-  <si>
     <t>FLOW_PRICE_008</t>
   </si>
   <si>
@@ -332,7 +332,7 @@
   "price_validation": 
   [
     {"booking_index": 0, "expected_amount": 1700000},
-    {"booking_index": 1, "expected_amount": 1700000}
+    {"booking_index": 1, "expected_amount": 1400000}
   ]
 }</t>
   </si>
@@ -342,10 +342,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -854,16 +854,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1018,6 +1018,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1025,9 +1028,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1565,20 +1565,20 @@
   <sheetPr/>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.171875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.2734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.0390625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="56.5078125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.2890625" style="1"/>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9238095238095" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1714285714286" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.2761904761905" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.0380952380952" style="1" customWidth="1"/>
+    <col min="7" max="7" width="56.5047619047619" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.2857142857143" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="24" customHeight="1" spans="1:7">
@@ -1604,7 +1604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="98" spans="1:7">
+    <row r="2" ht="94.5" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1623,11 +1623,11 @@
       <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" ht="98" spans="1:7">
+    <row r="3" ht="94.5" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1646,15 +1646,15 @@
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" ht="84" spans="1:7">
+    <row r="4" ht="94.5" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1669,22 +1669,22 @@
       <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" ht="84" spans="1:7">
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" ht="94.5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>11</v>
@@ -1692,22 +1692,22 @@
       <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" ht="84" spans="1:7">
+    <row r="6" ht="81" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
         <v>25</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>11</v>
@@ -1715,22 +1715,22 @@
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" ht="84" spans="1:7">
+      <c r="G6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" ht="94.5" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>11</v>
@@ -1738,22 +1738,22 @@
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" ht="84" spans="1:7">
+      <c r="G7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" ht="94.5" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="8" t="s">
         <v>33</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>11</v>
@@ -1761,15 +1761,15 @@
       <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" ht="84" spans="1:7">
+      <c r="G8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" ht="94.5" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1784,15 +1784,15 @@
       <c r="F9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" ht="84" spans="1:7">
+    <row r="10" ht="94.5" spans="1:7">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1807,15 +1807,15 @@
       <c r="F10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" ht="84" spans="1:7">
+    <row r="11" ht="94.5" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1830,15 +1830,15 @@
       <c r="F11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" ht="84" spans="1:7">
+    <row r="12" ht="94.5" spans="1:7">
       <c r="A12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1853,15 +1853,15 @@
       <c r="F12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" ht="84" spans="1:7">
+    <row r="13" ht="94.5" spans="1:7">
       <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1876,15 +1876,15 @@
       <c r="F13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" ht="84" spans="1:7">
+    <row r="14" ht="94.5" spans="1:7">
       <c r="A14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1899,15 +1899,15 @@
       <c r="F14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" ht="84" spans="1:7">
+      <c r="G14" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" ht="94.5" spans="1:7">
       <c r="A15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1922,15 +1922,15 @@
       <c r="F15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" ht="84" spans="1:7">
+    <row r="16" ht="94.5" spans="1:7">
       <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1945,15 +1945,15 @@
       <c r="F16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" ht="84" spans="1:7">
+      <c r="G16" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" ht="94.5" spans="1:7">
       <c r="A17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>66</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1968,15 +1968,15 @@
       <c r="F17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" ht="84" spans="1:7">
+    <row r="18" ht="94.5" spans="1:7">
       <c r="A18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1991,15 +1991,15 @@
       <c r="F18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" ht="84" spans="1:7">
+    <row r="19" ht="94.5" spans="1:7">
       <c r="A19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>72</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -2014,15 +2014,15 @@
       <c r="F19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" ht="84" spans="1:7">
+      <c r="G19" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" ht="94.5" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -2037,15 +2037,15 @@
       <c r="F20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" ht="84" spans="1:7">
+    <row r="21" ht="94.5" spans="1:7">
       <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -2060,15 +2060,15 @@
       <c r="F21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" ht="98" spans="1:7">
+      <c r="G21" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" ht="121.5" spans="1:7">
       <c r="A22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -2083,7 +2083,7 @@
       <c r="F22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="7" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>